<commit_message>
Wait for Parent Group Pickup
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/excel/data.rbac.xlsx
+++ b/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/excel/data.rbac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/vertx-zero/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA50145-50AD-B446-9375-B1D769CBE319}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4223DB42-46D3-8B4D-9812-3F284418DF21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22840" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
@@ -342,9 +342,6 @@
     <t>G31 - GROUP.SALE</t>
   </si>
   <si>
-    <t>本地分公司</t>
-  </si>
-  <si>
     <t>公司</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>G21 - GROUP.OUT</t>
   </si>
   <si>
-    <t>外地分公司</t>
-  </si>
-  <si>
     <t>G32 - GROUP.DESIGN</t>
   </si>
   <si>
@@ -508,13 +502,19 @@
   </si>
   <si>
     <t>部门列变更</t>
+  </si>
+  <si>
+    <t>本地支行</t>
+  </si>
+  <si>
+    <t>外地支行</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -546,6 +546,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -660,9 +668,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,12 +703,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -722,6 +721,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,6 +737,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1051,305 +1059,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE8EFB5-630A-0B48-8E56-AEAA85248043}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="43.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="15" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="59" style="6" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="6"/>
+    <col min="7" max="7" width="13.6640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="59" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="8" t="str">
+      <c r="B4" s="7" t="str">
         <f>A11</f>
         <v>8c148b72-7348-4d4e-b604-3b7d6053ac1e</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="8" t="str">
+      <c r="B5" s="7" t="str">
         <f>A12</f>
         <v>9744ae98-eac1-4825-b558-3e53c78940da</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="33"/>
+      <c r="F5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="12"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="12"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="F11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="34" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="F12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="33" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1357,233 +1365,233 @@
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" s="10" t="s">
+      <c r="E18" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="9" t="b">
+      <c r="E19" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="9" t="b">
+      <c r="E20" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F20" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="13"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B21" s="27" t="s">
+      <c r="A21" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E21" s="9" t="b">
+      <c r="E21" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F21" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="F21" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="13"/>
+      <c r="H21" s="12"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>113</v>
+      <c r="C25" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="str">
+      <c r="A27" s="7" t="str">
         <f>A18</f>
         <v>e501b47a-c08b-4c83-b12b-95ad82873e96</v>
       </c>
-      <c r="B27" s="24" t="str">
+      <c r="B27" s="21" t="str">
         <f>A11</f>
         <v>8c148b72-7348-4d4e-b604-3b7d6053ac1e</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="7" t="str">
         <f>A20</f>
         <v>89791ff1-dfe4-4906-b900-26df1ae01852</v>
       </c>
-      <c r="B28" s="24" t="str">
+      <c r="B28" s="21" t="str">
         <f>A11</f>
         <v>8c148b72-7348-4d4e-b604-3b7d6053ac1e</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="str">
+      <c r="A29" s="7" t="str">
         <f>A19</f>
         <v>cc884efe-b8dc-48dc-93b0-334b1926ad51</v>
       </c>
-      <c r="B29" s="24" t="str">
+      <c r="B29" s="21" t="str">
         <f>A12</f>
         <v>9744ae98-eac1-4825-b558-3e53c78940da</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1591,203 +1599,203 @@
       <c r="A32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G34" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="9" t="s">
+      <c r="D35" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F35" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" s="10" t="s">
+      <c r="F35" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E36" s="8" t="str">
+      <c r="D36" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" s="7" t="str">
         <f>A35</f>
         <v>c978f9e7-dc14-4c0e-b8ff-2d327a0c0be9</v>
       </c>
-      <c r="F36" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" s="10" t="s">
+      <c r="F36" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E37" s="26" t="str">
+      <c r="D37" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="23" t="str">
         <f>A36</f>
         <v>8e367b21-67bd-4c75-8058-5a0bc2d39d5c</v>
       </c>
-      <c r="F37" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" s="10" t="s">
+      <c r="F37" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="26" t="str">
+      <c r="D38" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="23" t="str">
         <f>A36</f>
         <v>8e367b21-67bd-4c75-8058-5a0bc2d39d5c</v>
       </c>
-      <c r="F38" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" s="10" t="s">
+      <c r="F38" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="10" t="s">
+      <c r="A39" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E39" s="26" t="str">
+      <c r="D39" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" s="23" t="str">
         <f>A35</f>
         <v>c978f9e7-dc14-4c0e-b8ff-2d327a0c0be9</v>
       </c>
-      <c r="F39" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="10" t="s">
+      <c r="F39" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="10" t="s">
+      <c r="A40" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" s="26" t="str">
+      <c r="D40" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="23" t="str">
         <f>A39</f>
         <v>d95fac7a-6586-4038-9d45-7b0844c7333c</v>
       </c>
-      <c r="F40" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="10" t="s">
+      <c r="F40" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1795,71 +1803,71 @@
       <c r="A43" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="22" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>113</v>
+      <c r="C44" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="str">
+      <c r="A46" s="23" t="str">
         <f>A36</f>
         <v>8e367b21-67bd-4c75-8058-5a0bc2d39d5c</v>
       </c>
-      <c r="B46" s="24" t="str">
+      <c r="B46" s="21" t="str">
         <f>A11</f>
         <v>8c148b72-7348-4d4e-b604-3b7d6053ac1e</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="str">
+      <c r="A47" s="7" t="str">
         <f>A38</f>
         <v>1b44b29a-4fcd-4996-bc0a-dd27231dab34</v>
       </c>
-      <c r="B47" s="24" t="str">
+      <c r="B47" s="21" t="str">
         <f>A11</f>
         <v>8c148b72-7348-4d4e-b604-3b7d6053ac1e</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="str">
+      <c r="A48" s="7" t="str">
         <f>A40</f>
         <v>658d7b7c-a024-4414-8367-25486a6f7797</v>
       </c>
-      <c r="B48" s="24" t="str">
+      <c r="B48" s="21" t="str">
         <f>A11</f>
         <v>8c148b72-7348-4d4e-b604-3b7d6053ac1e</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1867,97 +1875,123 @@
       <c r="A50" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="14" t="s">
-        <v>113</v>
+      <c r="C51" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="6" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="26" t="str">
+      <c r="A53" s="23" t="str">
         <f>A36</f>
         <v>8e367b21-67bd-4c75-8058-5a0bc2d39d5c</v>
       </c>
-      <c r="B53" s="24" t="str">
+      <c r="B53" s="21" t="str">
         <f>A19</f>
         <v>cc884efe-b8dc-48dc-93b0-334b1926ad51</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="str">
+      <c r="A54" s="23" t="str">
         <f>A46</f>
         <v>8e367b21-67bd-4c75-8058-5a0bc2d39d5c</v>
       </c>
-      <c r="B54" s="24" t="str">
+      <c r="B54" s="21" t="str">
         <f>A21</f>
         <v>2d335c9c-1547-4665-9643-6b0c7aaeb320</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="26" t="str">
+      <c r="A55" s="23" t="str">
         <f>A38</f>
         <v>1b44b29a-4fcd-4996-bc0a-dd27231dab34</v>
       </c>
-      <c r="B55" s="24" t="str">
+      <c r="B55" s="21" t="str">
         <f>A19</f>
         <v>cc884efe-b8dc-48dc-93b0-334b1926ad51</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="str">
+      <c r="A56" s="23" t="str">
         <f>A38</f>
         <v>1b44b29a-4fcd-4996-bc0a-dd27231dab34</v>
       </c>
-      <c r="B56" s="24" t="str">
+      <c r="B56" s="21" t="str">
         <f>A18</f>
         <v>e501b47a-c08b-4c83-b12b-95ad82873e96</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="26" t="str">
+      <c r="A57" s="23" t="str">
         <f>A40</f>
         <v>658d7b7c-a024-4414-8367-25486a6f7797</v>
       </c>
-      <c r="B57" s="24" t="str">
+      <c r="B57" s="21" t="str">
         <f>A20</f>
         <v>89791ff1-dfe4-4906-b900-26df1ae01852</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="23" t="str">
+        <f>A35</f>
+        <v>c978f9e7-dc14-4c0e-b8ff-2d327a0c0be9</v>
+      </c>
+      <c r="B58" s="21" t="str">
+        <f>A19</f>
+        <v>cc884efe-b8dc-48dc-93b0-334b1926ad51</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="23" t="str">
+        <f>A39</f>
+        <v>d95fac7a-6586-4038-9d45-7b0844c7333c</v>
+      </c>
+      <c r="B59" s="21" t="str">
+        <f>A18</f>
+        <v>e501b47a-c08b-4c83-b12b-95ad82873e96</v>
+      </c>
+      <c r="C59" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1987,9 +2021,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.1640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="39.1640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="52.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="1" customWidth="1"/>
@@ -1999,273 +2033,273 @@
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="B4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" s="14" t="s">
+      <c r="E4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="E6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="E8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="29" t="s">
+      <c r="E9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="D10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="29" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="D11" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="29" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="D12" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="29" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="D13" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="29" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="D14" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" s="29" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="D15" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="29" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E14" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="E15" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="D16" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="E16" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="E16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2273,168 +2307,168 @@
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="C21" s="25" t="s">
+      <c r="B21" s="25" t="s">
         <v>146</v>
       </c>
+      <c r="C21" s="22" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="20"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="23"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C23" s="23"/>
+      <c r="C23" s="20"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="str">
+      <c r="A24" s="23" t="str">
         <f>'DATA-WHO'!A$18</f>
         <v>e501b47a-c08b-4c83-b12b-95ad82873e96</v>
       </c>
-      <c r="B24" s="24" t="str">
+      <c r="B24" s="21" t="str">
         <f>A6</f>
         <v>bf4f20d0-cc24-47c6-8d1e-c81bfc3772a3</v>
       </c>
-      <c r="C24" s="23"/>
+      <c r="C24" s="20"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="str">
+      <c r="A25" s="23" t="str">
         <f>'DATA-WHO'!A$18</f>
         <v>e501b47a-c08b-4c83-b12b-95ad82873e96</v>
       </c>
-      <c r="B25" s="24" t="str">
+      <c r="B25" s="21" t="str">
         <f>A7</f>
         <v>f6d06a71-5acb-4a2e-8799-67b6a17d482e</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="str">
+      <c r="A26" s="23" t="str">
         <f>'DATA-WHO'!A$18</f>
         <v>e501b47a-c08b-4c83-b12b-95ad82873e96</v>
       </c>
-      <c r="B26" s="24" t="str">
+      <c r="B26" s="21" t="str">
         <f>A8</f>
         <v>e71c22da-bedc-46b2-9fc2-0123b8ba8fdc</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="str">
+      <c r="A27" s="23" t="str">
         <f>'DATA-WHO'!A$18</f>
         <v>e501b47a-c08b-4c83-b12b-95ad82873e96</v>
       </c>
-      <c r="B27" s="24" t="str">
+      <c r="B27" s="21" t="str">
         <f>A9</f>
         <v>1ec73d5f-26e4-481b-aed8-7236ef0fb101</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="str">
+      <c r="A28" s="23" t="str">
         <f>'DATA-WHO'!A$18</f>
         <v>e501b47a-c08b-4c83-b12b-95ad82873e96</v>
       </c>
-      <c r="B28" s="24" t="str">
+      <c r="B28" s="21" t="str">
         <f>A10</f>
         <v>45831b92-a796-482d-a419-28dd7e1d0a2e</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="str">
+      <c r="A29" s="23" t="str">
         <f>'DATA-WHO'!A$20</f>
         <v>89791ff1-dfe4-4906-b900-26df1ae01852</v>
       </c>
-      <c r="B29" s="24" t="str">
+      <c r="B29" s="21" t="str">
         <f>A6</f>
         <v>bf4f20d0-cc24-47c6-8d1e-c81bfc3772a3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="str">
+      <c r="A30" s="23" t="str">
         <f>'DATA-WHO'!A$20</f>
         <v>89791ff1-dfe4-4906-b900-26df1ae01852</v>
       </c>
-      <c r="B30" s="24" t="str">
+      <c r="B30" s="21" t="str">
         <f>A11</f>
         <v>6ca8c035-8bba-4d4d-aadd-7d06bf4b0a5a</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="str">
+      <c r="A31" s="23" t="str">
         <f>'DATA-WHO'!A$20</f>
         <v>89791ff1-dfe4-4906-b900-26df1ae01852</v>
       </c>
-      <c r="B31" s="24" t="str">
+      <c r="B31" s="21" t="str">
         <f>A12</f>
         <v>59c45dc0-eed5-42dc-baf5-f10fa0e02827</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="str">
+      <c r="A32" s="23" t="str">
         <f>'DATA-WHO'!A$19</f>
         <v>cc884efe-b8dc-48dc-93b0-334b1926ad51</v>
       </c>
-      <c r="B32" s="24" t="str">
+      <c r="B32" s="21" t="str">
         <f>A6</f>
         <v>bf4f20d0-cc24-47c6-8d1e-c81bfc3772a3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="str">
+      <c r="A33" s="23" t="str">
         <f>'DATA-WHO'!A$19</f>
         <v>cc884efe-b8dc-48dc-93b0-334b1926ad51</v>
       </c>
-      <c r="B33" s="24" t="str">
+      <c r="B33" s="21" t="str">
         <f>A13</f>
         <v>d17d873f-65f1-49e3-99a3-30733bf84d1b</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="str">
+      <c r="A34" s="23" t="str">
         <f>'DATA-WHO'!A$19</f>
         <v>cc884efe-b8dc-48dc-93b0-334b1926ad51</v>
       </c>
-      <c r="B34" s="24" t="str">
+      <c r="B34" s="21" t="str">
         <f>A14</f>
         <v>e08b418c-0557-453c-8cdf-5c0278ac7c26</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="str">
+      <c r="A35" s="23" t="str">
         <f>'DATA-WHO'!A$21</f>
         <v>2d335c9c-1547-4665-9643-6b0c7aaeb320</v>
       </c>
-      <c r="B35" s="24" t="str">
+      <c r="B35" s="21" t="str">
         <f>A6</f>
         <v>bf4f20d0-cc24-47c6-8d1e-c81bfc3772a3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="str">
+      <c r="A36" s="23" t="str">
         <f>'DATA-WHO'!A$21</f>
         <v>2d335c9c-1547-4665-9643-6b0c7aaeb320</v>
       </c>
-      <c r="B36" s="24" t="str">
+      <c r="B36" s="21" t="str">
         <f>A15</f>
         <v>885d659d-ffc1-4d36-bc66-1a5fa75d07bf</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="str">
+      <c r="A37" s="23" t="str">
         <f>'DATA-WHO'!A$21</f>
         <v>2d335c9c-1547-4665-9643-6b0c7aaeb320</v>
       </c>
-      <c r="B37" s="24" t="str">
+      <c r="B37" s="21" t="str">
         <f>A16</f>
         <v>a50e1e66-737d-4270-b49e-c2e343c3fea3</v>
       </c>

</xml_diff>

<commit_message>
Dept Testing for Authorization
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/excel/data.rbac.xlsx
+++ b/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/excel/data.rbac.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/vertx-zero/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4223DB42-46D3-8B4D-9812-3F284418DF21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0897FA-5535-8944-AB5E-B4D1D98C7029}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22840" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22840" activeTab="1" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-WHO" sheetId="1" r:id="rId1"/>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId2"/>
+    <sheet name="DATA-RESOURCE" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -723,6 +724,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -737,12 +744,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1061,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE8EFB5-630A-0B48-8E56-AEAA85248043}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
@@ -1087,14 +1088,14 @@
       <c r="B1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
     </row>
@@ -1165,7 +1166,7 @@
       <c r="D4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="8" t="b">
         <v>1</v>
       </c>
@@ -1190,7 +1191,7 @@
       <c r="D5" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="8" t="b">
         <v>1</v>
       </c>
@@ -1222,16 +1223,16 @@
       <c r="B8" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -1325,7 +1326,7 @@
       <c r="I11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="29" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1357,7 +1358,7 @@
       <c r="I12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="J12" s="28" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1368,13 +1369,13 @@
       <c r="B15" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
@@ -1602,13 +1603,13 @@
       <c r="B32" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="31"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -2015,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
   <dimension ref="A3:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2036,12 +2037,12 @@
       <c r="B3" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -2480,4 +2481,16 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26D6822-B54B-7D4E-BA6F-6D516D4A4E04}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>